<commit_message>
create additional 3 column done and get bankname method success
</commit_message>
<xml_diff>
--- a/ClearingFramework/functions/Данс.xlsx
+++ b/ClearingFramework/functions/Данс.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\altanbagana.n\Documents\GitHub\ClearingFramework\ClearingFramework\functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91137B32-29A0-47AE-B9CF-215908916129}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34142E0A-0624-40D2-BD5A-9216B53D64D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5610" yWindow="3765" windowWidth="24585" windowHeight="12360" xr2:uid="{B4FE0422-C962-4475-929B-8BFC1E41559F}"/>
+    <workbookView xWindow="13230" yWindow="3945" windowWidth="24585" windowHeight="12360" xr2:uid="{B4FE0422-C962-4475-929B-8BFC1E41559F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="53">
   <si>
     <t>lname</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>denchinPercent</t>
+  </si>
+  <si>
+    <t>bank</t>
+  </si>
+  <si>
+    <t>bankAccName</t>
+  </si>
+  <si>
+    <t>bankAccount</t>
   </si>
 </sst>
 </file>
@@ -553,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E8D0FF5-F7FB-46A2-BF04-B810356663A3}">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,15 +573,17 @@
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="15.140625" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" customWidth="1"/>
     <col min="9" max="9" width="6.42578125" customWidth="1"/>
     <col min="10" max="10" width="14.140625" customWidth="1"/>
     <col min="13" max="13" width="15.5703125" customWidth="1"/>
     <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -621,8 +632,17 @@
       <c r="P1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>87979</v>
       </c>
@@ -671,8 +691,17 @@
       <c r="P2">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2">
+        <v>1232155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>87980</v>
       </c>
@@ -721,8 +750,17 @@
       <c r="P3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S3">
+        <v>54674567</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>87981</v>
       </c>
@@ -771,8 +809,17 @@
       <c r="P4">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>15</v>
+      </c>
+      <c r="S4">
+        <v>108116979</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>87982</v>
       </c>
@@ -821,8 +868,17 @@
       <c r="P5">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5">
+        <v>161559391</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>87983</v>
       </c>
@@ -871,8 +927,17 @@
       <c r="P6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6" t="s">
+        <v>15</v>
+      </c>
+      <c r="S6">
+        <v>215001803</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>87984</v>
       </c>
@@ -921,8 +986,17 @@
       <c r="P7">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q7">
+        <v>6</v>
+      </c>
+      <c r="R7" t="s">
+        <v>16</v>
+      </c>
+      <c r="S7">
+        <v>268444215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>87985</v>
       </c>
@@ -971,8 +1045,17 @@
       <c r="P8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <v>7</v>
+      </c>
+      <c r="R8" t="s">
+        <v>15</v>
+      </c>
+      <c r="S8">
+        <v>321886627</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>87986</v>
       </c>
@@ -1021,8 +1104,17 @@
       <c r="P9">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>8</v>
+      </c>
+      <c r="R9" t="s">
+        <v>16</v>
+      </c>
+      <c r="S9">
+        <v>375329039</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>87987</v>
       </c>
@@ -1071,8 +1163,17 @@
       <c r="P10">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <v>9</v>
+      </c>
+      <c r="R10" t="s">
+        <v>15</v>
+      </c>
+      <c r="S10">
+        <v>428771451</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>87988</v>
       </c>
@@ -1121,8 +1222,17 @@
       <c r="P11">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q11">
+        <v>10</v>
+      </c>
+      <c r="R11" t="s">
+        <v>16</v>
+      </c>
+      <c r="S11">
+        <v>482213863</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>87989</v>
       </c>
@@ -1171,8 +1281,17 @@
       <c r="P12">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q12">
+        <v>11</v>
+      </c>
+      <c r="R12" t="s">
+        <v>15</v>
+      </c>
+      <c r="S12">
+        <v>535656275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>87990</v>
       </c>
@@ -1221,8 +1340,17 @@
       <c r="P13">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q13">
+        <v>12</v>
+      </c>
+      <c r="R13" t="s">
+        <v>16</v>
+      </c>
+      <c r="S13">
+        <v>589098687</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>87991</v>
       </c>
@@ -1271,8 +1399,17 @@
       <c r="P14">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q14">
+        <v>13</v>
+      </c>
+      <c r="R14" t="s">
+        <v>15</v>
+      </c>
+      <c r="S14">
+        <v>642541099</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>87992</v>
       </c>
@@ -1321,8 +1458,17 @@
       <c r="P15">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <v>14</v>
+      </c>
+      <c r="R15" t="s">
+        <v>16</v>
+      </c>
+      <c r="S15">
+        <v>695983511</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>87993</v>
       </c>
@@ -1371,8 +1517,17 @@
       <c r="P16">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <v>15</v>
+      </c>
+      <c r="R16" t="s">
+        <v>15</v>
+      </c>
+      <c r="S16">
+        <v>749425923</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>87994</v>
       </c>
@@ -1421,8 +1576,17 @@
       <c r="P17">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <v>16</v>
+      </c>
+      <c r="R17" t="s">
+        <v>16</v>
+      </c>
+      <c r="S17">
+        <v>802868335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>87995</v>
       </c>
@@ -1471,8 +1635,17 @@
       <c r="P18">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <v>17</v>
+      </c>
+      <c r="R18" t="s">
+        <v>15</v>
+      </c>
+      <c r="S18">
+        <v>856310747</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>87996</v>
       </c>
@@ -1521,8 +1694,17 @@
       <c r="P19">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q19">
+        <v>18</v>
+      </c>
+      <c r="R19" t="s">
+        <v>16</v>
+      </c>
+      <c r="S19">
+        <v>909753159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>87997</v>
       </c>
@@ -1571,8 +1753,17 @@
       <c r="P20">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q20">
+        <v>19</v>
+      </c>
+      <c r="R20" t="s">
+        <v>15</v>
+      </c>
+      <c r="S20">
+        <v>963195571</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>87998</v>
       </c>
@@ -1621,8 +1812,17 @@
       <c r="P21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q21">
+        <v>20</v>
+      </c>
+      <c r="R21" t="s">
+        <v>16</v>
+      </c>
+      <c r="S21">
+        <v>1016637983</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>87999</v>
       </c>
@@ -1671,8 +1871,17 @@
       <c r="P22">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <v>21</v>
+      </c>
+      <c r="R22" t="s">
+        <v>15</v>
+      </c>
+      <c r="S22">
+        <v>1070080395</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>88000</v>
       </c>
@@ -1721,8 +1930,17 @@
       <c r="P23">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q23">
+        <v>22</v>
+      </c>
+      <c r="R23" t="s">
+        <v>16</v>
+      </c>
+      <c r="S23">
+        <v>1123522807</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>88001</v>
       </c>
@@ -1771,8 +1989,17 @@
       <c r="P24">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q24">
+        <v>23</v>
+      </c>
+      <c r="R24" t="s">
+        <v>15</v>
+      </c>
+      <c r="S24">
+        <v>1176965219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>88002</v>
       </c>
@@ -1821,8 +2048,17 @@
       <c r="P25">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q25">
+        <v>24</v>
+      </c>
+      <c r="R25" t="s">
+        <v>16</v>
+      </c>
+      <c r="S25">
+        <v>1230407631</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>88003</v>
       </c>
@@ -1871,8 +2107,17 @@
       <c r="P26">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q26">
+        <v>25</v>
+      </c>
+      <c r="R26" t="s">
+        <v>15</v>
+      </c>
+      <c r="S26">
+        <v>1283850043</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>88004</v>
       </c>
@@ -1921,8 +2166,17 @@
       <c r="P27">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q27">
+        <v>26</v>
+      </c>
+      <c r="R27" t="s">
+        <v>16</v>
+      </c>
+      <c r="S27">
+        <v>1337292455</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>88005</v>
       </c>
@@ -1971,8 +2225,17 @@
       <c r="P28">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q28">
+        <v>27</v>
+      </c>
+      <c r="R28" t="s">
+        <v>15</v>
+      </c>
+      <c r="S28">
+        <v>1390734867</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>88006</v>
       </c>
@@ -2021,8 +2284,17 @@
       <c r="P29">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q29">
+        <v>28</v>
+      </c>
+      <c r="R29" t="s">
+        <v>16</v>
+      </c>
+      <c r="S29">
+        <v>1444177279</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>88007</v>
       </c>
@@ -2071,8 +2343,17 @@
       <c r="P30">
         <v>20</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q30">
+        <v>29</v>
+      </c>
+      <c r="R30" t="s">
+        <v>15</v>
+      </c>
+      <c r="S30">
+        <v>1497619691</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>88008</v>
       </c>
@@ -2121,8 +2402,17 @@
       <c r="P31">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q31">
+        <v>30</v>
+      </c>
+      <c r="R31" t="s">
+        <v>16</v>
+      </c>
+      <c r="S31">
+        <v>1551062103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>88009</v>
       </c>
@@ -2170,6 +2460,15 @@
       </c>
       <c r="P32">
         <v>20</v>
+      </c>
+      <c r="Q32">
+        <v>31</v>
+      </c>
+      <c r="R32" t="s">
+        <v>15</v>
+      </c>
+      <c r="S32">
+        <v>1604504515</v>
       </c>
     </row>
   </sheetData>

</xml_diff>